<commit_message>
Update README, add hackster.io project  link, and add missing diode to BOM
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Rob\Dropbox\Dropbox\rob\Repository\MailNotifier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E84487AF-23CD-439B-B215-6491C498DF47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15361787-C4C2-42DC-A70B-12B3F538B218}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="17970" xr2:uid="{ECF97B3F-5AE9-4566-9E2E-ADFCD7651E86}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Item</t>
   </si>
@@ -154,6 +154,15 @@
   </si>
   <si>
     <t>Purchase URL (examplse - available at multiple outlets)</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>1N4007</t>
+  </si>
+  <si>
+    <t>https://octopart.com/1n4007-t-diodes+inc.-55389582?r=sp&amp;s=AmIHlQKgSlimIGmMg_WMyg</t>
   </si>
 </sst>
 </file>
@@ -220,8 +229,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{980C2DB9-13C0-4BAB-B297-1844E42CE748}" name="Table1" displayName="Table1" ref="A1:D16" totalsRowShown="0">
-  <autoFilter ref="A1:D16" xr:uid="{9F54C7D5-49C7-4F4B-98B9-4CBF3D52228A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{980C2DB9-13C0-4BAB-B297-1844E42CE748}" name="Table1" displayName="Table1" ref="A1:D17" totalsRowShown="0">
+  <autoFilter ref="A1:D17" xr:uid="{9F54C7D5-49C7-4F4B-98B9-4CBF3D52228A}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{AE6E1C4A-08F8-4DC1-A189-8CF31FA9A245}" name="Item"/>
     <tableColumn id="2" xr3:uid="{898C35AC-A349-443A-B89C-56D27D323448}" name="Qty"/>
@@ -529,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1EEDC6-B1A6-4167-8F8B-F2256C571711}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,31 +724,45 @@
       <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>41</v>
       </c>
     </row>
@@ -749,10 +772,11 @@
     <hyperlink ref="D7" r:id="rId2" xr:uid="{16600D15-4BF1-4C99-8AA4-CE00C904270E}"/>
     <hyperlink ref="D5" r:id="rId3" xr:uid="{C8F9DCE2-8A8E-4635-86C9-CDDC7B74DAFB}"/>
     <hyperlink ref="D6" r:id="rId4" xr:uid="{D1476AC3-DAB6-4DE5-9AF7-B284E5EA7102}"/>
+    <hyperlink ref="D13" r:id="rId5" xr:uid="{7F6FDFBD-AACB-41F5-A2FA-B61EE1237CFE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>